<commit_message>
committing the probability of the whole data set
</commit_message>
<xml_diff>
--- a/root/Testing/Probability of Hit.xlsx
+++ b/root/Testing/Probability of Hit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="121">
   <si>
     <t xml:space="preserve">Test number </t>
   </si>
@@ -372,6 +372,24 @@
   </si>
   <si>
     <t>33 0.876</t>
+  </si>
+  <si>
+    <t>28 0.451</t>
+  </si>
+  <si>
+    <t>29 0.560</t>
+  </si>
+  <si>
+    <t>30 0.554</t>
+  </si>
+  <si>
+    <t>31 0.614</t>
+  </si>
+  <si>
+    <t>32 0.751</t>
+  </si>
+  <si>
+    <t>33 0.880</t>
   </si>
 </sst>
 </file>
@@ -729,7 +747,7 @@
   <dimension ref="B2:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1409,8 +1427,36 @@
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B21" s="3"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="3">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>

</xml_diff>